<commit_message>
uploading function of attributed program under plan and budget
</commit_message>
<xml_diff>
--- a/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
+++ b/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
@@ -467,6 +467,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -486,24 +504,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -816,12 +816,13 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="25.88671875" style="3" customWidth="1"/>
     <col min="4" max="5" width="25.88671875" style="12" customWidth="1"/>
     <col min="6" max="6" width="25.88671875" style="7" customWidth="1"/>
@@ -838,68 +839,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="20" t="s">
+      <c r="O1" s="24"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
       <c r="N2" s="2" t="s">
         <v>4</v>
       </c>
@@ -909,7 +910,7 @@
       <c r="P2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="21"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -919,12 +920,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:Q2"/>
@@ -934,6 +929,12 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" orientation="landscape" r:id="rId1"/>
@@ -944,13 +945,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="25.88671875" style="3" customWidth="1"/>
     <col min="4" max="5" width="25.88671875" style="12" customWidth="1"/>
     <col min="6" max="6" width="25.88671875" style="7" customWidth="1"/>
@@ -967,68 +969,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="20" t="s">
+      <c r="O1" s="24"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
       <c r="N2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1038,7 +1040,7 @@
       <c r="P2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="21"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -1089,7 +1091,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
@@ -1137,12 +1139,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
@@ -1152,6 +1148,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
attributed programs of accomplishment report import modules
</commit_message>
<xml_diff>
--- a/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
+++ b/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>GAD Objective</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Starte Here</t>
+  </si>
+  <si>
+    <t>GAD Plan and Budget</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +253,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,13 +276,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,14 +439,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -467,6 +480,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -479,35 +498,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,128 +832,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="25.88671875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="27.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.21875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="34.44140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="25.88671875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" style="10" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" style="10" customWidth="1"/>
-    <col min="17" max="17" width="13.21875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="25.88671875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="34.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="25.88671875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:17" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+    </row>
+    <row r="2" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="O2" s="25"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="2" t="s">
+    <row r="3" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="27"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="Q3" s="29"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L4" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" orientation="landscape" r:id="rId1"/>
@@ -943,217 +985,239 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="25.88671875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="27.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.21875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="34.44140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="25.88671875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" style="10" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" style="10" customWidth="1"/>
-    <col min="17" max="17" width="13.21875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="25.88671875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="34.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="25.88671875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:17" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+    </row>
+    <row r="2" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="O2" s="25"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="2" t="s">
+    <row r="3" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="27"/>
-    </row>
-    <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+      <c r="Q3" s="29"/>
+    </row>
+    <row r="4" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L4" s="7">
         <v>43497</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M4" s="8">
         <v>43524</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N4" s="9">
         <v>100000</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+    <row r="5" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L5" s="8">
         <v>43534</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M5" s="8">
         <v>43541</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N5" s="9">
         <v>258000</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q5" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="H11" s="4"/>
-      <c r="I11" s="13"/>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H12" s="3"/>
+      <c r="I12" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" orientation="landscape" r:id="rId1"/>
@@ -1175,17 +1239,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
print preview for gad plan and budget
</commit_message>
<xml_diff>
--- a/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
+++ b/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
+    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ACTUAL DATA SHEET" sheetId="10" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>GAD Objective</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>GAD Plan and Budget</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -480,53 +483,53 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,9 +837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,25 +862,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
     </row>
     <row r="2" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -886,7 +889,7 @@
       <c r="B2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="16" t="s">
@@ -898,25 +901,25 @@
       <c r="F2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="24" t="s">
@@ -931,27 +934,27 @@
     <row r="3" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
-      <c r="C3" s="23"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="28" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="28" t="s">
+      <c r="O3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="29"/>
+      <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -987,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,25 +1014,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
     </row>
     <row r="2" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -1038,7 +1041,7 @@
       <c r="B2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="16" t="s">
@@ -1050,25 +1053,25 @@
       <c r="F2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="24" t="s">
@@ -1083,27 +1086,27 @@
     <row r="3" spans="1:17" ht="68.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
-      <c r="C3" s="23"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="28" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="28" t="s">
+      <c r="O3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="29"/>
+      <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
@@ -1126,6 +1129,9 @@
       </c>
       <c r="G4" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>53</v>
@@ -1239,10 +1245,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="29"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changes in template of plan
</commit_message>
<xml_diff>
--- a/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
+++ b/frontend/web/uploads/template/excel/GAD-Plan-Budget-Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" activeTab="1"/>
+    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
   </bookViews>
   <sheets>
     <sheet name="ACTUAL DATA SHEET" sheetId="10" r:id="rId1"/>
@@ -837,9 +837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>